<commit_message>
2 files has been updated
</commit_message>
<xml_diff>
--- a/Activity Tracker.xlsx
+++ b/Activity Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d322042a4f68d17/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonali\OneDrive\Desktop\git_prac_2\second_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{F988E72B-712A-4DE2-8A45-44279D8328E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E5EBB86-4591-477B-A568-E15DE50D4C26}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA358D7-8DF5-4C63-A5FF-80AAC3234F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{21772E3D-7E4C-4E4C-8708-6D5C382999AF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{21772E3D-7E4C-4E4C-8708-6D5C382999AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="61">
   <si>
     <t>Sr.No</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>After Each Month's 20 th Date</t>
+  </si>
+  <si>
+    <t>Its finished now</t>
   </si>
 </sst>
 </file>
@@ -572,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57748AAC-3B50-4CA3-8E1B-368C15296C26}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,6 +1081,14 @@
         <v>28</v>
       </c>
     </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>